<commit_message>
[2020-09-15 10:53] 추천알고리즘 90% 완성
</commit_message>
<xml_diff>
--- a/dataWork/controller/test_reco.xlsx
+++ b/dataWork/controller/test_reco.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\kjy\pics\dataWork\controller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{462F62AE-4891-4ACE-B158-131E60B8E84D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D69EB1C8-1D64-4B45-85AE-48A986A4D4EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8460" yWindow="1260" windowWidth="17280" windowHeight="8964" xr2:uid="{BAD44B8A-84D6-43B5-A9F4-F6E4D4B6150C}"/>
+    <workbookView xWindow="5124" yWindow="2004" windowWidth="17280" windowHeight="8964" xr2:uid="{BAD44B8A-84D6-43B5-A9F4-F6E4D4B6150C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -411,7 +411,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:C20"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -436,7 +436,7 @@
       </c>
       <c r="C2">
         <f ca="1">RANDBETWEEN(0,5)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
@@ -447,8 +447,8 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C20" ca="1" si="0">RANDBETWEEN(0,5)</f>
-        <v>4</v>
+        <f t="shared" ref="C3:C11" ca="1" si="0">RANDBETWEEN(0,5)</f>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
@@ -460,7 +460,7 @@
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
@@ -472,7 +472,7 @@
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
@@ -484,7 +484,7 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
@@ -520,7 +520,7 @@
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
@@ -532,19 +532,19 @@
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>